<commit_message>
Documentado el segundo anexo (Especificación de requisitos) y añadidos pequeños cambios y actualizaciones en la memoria.
</commit_message>
<xml_diff>
--- a/doc/latex/Scrum.xlsx
+++ b/doc/latex/Scrum.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16215" windowHeight="7530" firstSheet="5" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16215" windowHeight="7530" firstSheet="6" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 0" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,8 @@
     <sheet name="Sprint 9" sheetId="11" r:id="rId10"/>
     <sheet name="Sprint 10" sheetId="12" r:id="rId11"/>
     <sheet name="Sprint 11" sheetId="13" r:id="rId12"/>
-    <sheet name="Resumen" sheetId="14" r:id="rId13"/>
+    <sheet name="Sprint 12" sheetId="15" r:id="rId13"/>
+    <sheet name="Resumen" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="232">
   <si>
     <t>Elegir el lenguaje de programación</t>
   </si>
@@ -690,6 +691,48 @@
   </si>
   <si>
     <t>Porcentaje</t>
+  </si>
+  <si>
+    <t>Añadir carpeta con el framework de inteligencia artificial y sus dependencias.</t>
+  </si>
+  <si>
+    <t>Sprint 12 (08/06/17 - 14/06/17)</t>
+  </si>
+  <si>
+    <t>Día 1 (08/06/17)</t>
+  </si>
+  <si>
+    <t>Día 2 (09/06/17)</t>
+  </si>
+  <si>
+    <t>Día 3 (10/06/17)</t>
+  </si>
+  <si>
+    <t>Día 4 (11/06/17)</t>
+  </si>
+  <si>
+    <t>Día 5 (12/06/17)</t>
+  </si>
+  <si>
+    <t>Día 6 (13/06/17)</t>
+  </si>
+  <si>
+    <t>Día 7 (14/06/17)</t>
+  </si>
+  <si>
+    <t>Añadir documento de licencia GNU GPL.</t>
+  </si>
+  <si>
+    <t>Documentar el primer anexo (manual).</t>
+  </si>
+  <si>
+    <t>Añadir recursos necesarios para su ejecución.</t>
+  </si>
+  <si>
+    <t>Corregir formato en la opción de exportar tabla en xls.</t>
+  </si>
+  <si>
+    <t>Documentar el segundo anexo (especificación de requisitos).</t>
   </si>
 </sst>
 </file>
@@ -987,15 +1030,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="7" borderId="11" xfId="6" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="6" applyBorder="1" applyAlignment="1">
@@ -1040,6 +1074,15 @@
     <xf numFmtId="1" fontId="1" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="7" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Énfasis3" xfId="5" builtinId="38"/>
@@ -3476,6 +3519,583 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>Sprint 12</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 12'!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Restante</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 12'!$B$3:$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Total Horas</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Día 1 (08/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Día 2 (09/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Día 3 (10/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Día 4 (11/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Día 5 (12/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Día 6 (13/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Día 7 (14/06/17)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 12'!$B$10:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9422-47A5-8F59-AB2E84FB9119}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 12'!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 12'!$B$3:$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Total Horas</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Día 1 (08/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Día 2 (09/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Día 3 (10/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Día 4 (11/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Día 5 (12/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Día 6 (13/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Día 7 (14/06/17)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 12'!$B$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.142857142857142</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.785714285714285</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.428571428571427</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.071428571428569</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.7142857142857117</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.3571428571428545</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9422-47A5-8F59-AB2E84FB9119}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="404108848"/>
+        <c:axId val="404106880"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="404108848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Dias</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="404106880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="404106880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Horas</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="404108848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
               <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="50" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
@@ -3724,16 +4344,16 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>6.8174583828132643E-2</c:v>
+                  <c:v>0.23547799304257364</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.4600190859508185E-2</c:v>
+                  <c:v>3.6467829974119147E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.7164701515357124E-2</c:v>
+                  <c:v>8.2052617441768089E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7900605237970022</c:v>
+                  <c:v>0.64600155954153915</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8851,6 +9471,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -11184,6 +11844,509 @@
 </file>
 
 <file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="258">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -16075,6 +17238,93 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
+      <xdr:colOff>19053</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89A32AAD-34EC-40CE-BFA2-F0FD71195F13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>372364</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>151530</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8E0048D-02F5-48A2-A201-4E77346ED138}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6086475" y="2752725"/>
+          <a:ext cx="5858764" cy="3151905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -16110,23 +17360,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>393589</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>12589</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>41006</xdr:rowOff>
+      <xdr:rowOff>88631</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
+        <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BB61A08-DB1C-4220-AD42-B82880739A10}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98A57A69-B128-4DE9-A777-101AE63D61BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16142,7 +17392,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4743450" y="1857375"/>
+          <a:off x="5124450" y="1905000"/>
           <a:ext cx="4584589" cy="2755631"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -17165,16 +18415,16 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="42"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="68"/>
       <c r="L2" s="3">
         <v>1</v>
       </c>
@@ -17504,23 +18754,23 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="40" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="66" t="s">
         <v>175</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="42"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="68"/>
     </row>
     <row r="3" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="44"/>
-      <c r="B3" s="45" t="s">
+      <c r="A3" s="41"/>
+      <c r="B3" s="42" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="21" t="s">
@@ -17570,24 +18820,24 @@
       <c r="J4" s="10"/>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="48" t="s">
+    <row r="5" spans="1:13" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="B5" s="49">
+      <c r="B5" s="46">
         <v>0.5</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49">
+      <c r="C5" s="46"/>
+      <c r="D5" s="46">
         <v>0.75</v>
       </c>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="50"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="47"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
@@ -17608,24 +18858,24 @@
       <c r="J6" s="13"/>
       <c r="K6" s="14"/>
     </row>
-    <row r="7" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
+    <row r="7" spans="1:13" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="49">
+      <c r="B7" s="46">
         <v>0.5</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49">
+      <c r="C7" s="46"/>
+      <c r="D7" s="46">
         <v>0.75</v>
       </c>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="50"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="47"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
@@ -17646,24 +18896,24 @@
       <c r="J8" s="13"/>
       <c r="K8" s="14"/>
     </row>
-    <row r="9" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="48" t="s">
+    <row r="9" spans="1:13" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="B9" s="49">
+      <c r="B9" s="46">
         <v>1</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49">
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46">
         <v>2</v>
       </c>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="50"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="47"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
@@ -17684,24 +18934,24 @@
       <c r="J10" s="13"/>
       <c r="K10" s="14"/>
     </row>
-    <row r="11" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
+    <row r="11" spans="1:13" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="45" t="s">
         <v>170</v>
       </c>
-      <c r="B11" s="49">
+      <c r="B11" s="46">
         <v>2</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49">
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46">
         <v>3</v>
       </c>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="50"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="47"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
@@ -17722,24 +18972,24 @@
       <c r="J12" s="13"/>
       <c r="K12" s="14"/>
     </row>
-    <row r="13" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="48" t="s">
+    <row r="13" spans="1:13" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="45" t="s">
         <v>172</v>
       </c>
-      <c r="B13" s="49">
+      <c r="B13" s="46">
         <v>1</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49">
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46">
         <v>2</v>
       </c>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="50"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="47"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
@@ -17760,22 +19010,22 @@
       <c r="J14" s="13"/>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" spans="1:13" s="51" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="48" t="s">
+    <row r="15" spans="1:13" s="48" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="45" t="s">
         <v>174</v>
       </c>
-      <c r="B15" s="49">
+      <c r="B15" s="46">
         <v>3</v>
       </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="50">
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="47">
         <v>4</v>
       </c>
     </row>
@@ -17788,39 +19038,39 @@
         <v>13</v>
       </c>
       <c r="C16" s="16">
-        <f>IF(B16-SUM(C4:C15)&gt;0,B16-SUM(C4:C15),0)</f>
+        <f t="shared" ref="C16:I16" si="0">IF(B16-SUM(C4:C15)&gt;0,B16-SUM(C4:C15),0)</f>
         <v>13</v>
       </c>
       <c r="D16" s="16">
-        <f>IF(C16-SUM(D4:D15)&gt;0,C16-SUM(D4:D15),0)</f>
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
       <c r="E16" s="16">
-        <f>IF(D16-SUM(E4:E15)&gt;0,D16-SUM(E4:E15),0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F16" s="16">
-        <f>IF(E16-SUM(F4:F15)&gt;0,E16-SUM(F4:F15),0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G16" s="16">
-        <f>IF(F16-SUM(G4:G15)&gt;0,F16-SUM(G4:G15),0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H16" s="16">
-        <f>IF(G16-SUM(H4:H15)&gt;0,G16-SUM(H4:H15),0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I16" s="16">
-        <f>IF(H16-SUM(I4:I15)&gt;0,H16-SUM(I4:I15),0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J16" s="16">
-        <f t="shared" ref="J16:K16" si="0">IF(I16-SUM(J4:J15)&gt;0,I16-SUM(J4:J15),0)</f>
+        <f t="shared" ref="J16:K16" si="1">IF(I16-SUM(J4:J15)&gt;0,I16-SUM(J4:J15),0)</f>
         <v>0</v>
       </c>
       <c r="K16" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L16" s="34" t="s">
@@ -17839,39 +19089,39 @@
         <v>13</v>
       </c>
       <c r="C17" s="19">
-        <f>B17-($B$17/COUNTA($C$3:$K$3))</f>
+        <f t="shared" ref="C17:I17" si="2">B17-($B$17/COUNTA($C$3:$K$3))</f>
         <v>11.555555555555555</v>
       </c>
       <c r="D17" s="19">
-        <f>C17-($B$17/COUNTA($C$3:$K$3))</f>
+        <f t="shared" si="2"/>
         <v>10.111111111111111</v>
       </c>
       <c r="E17" s="19">
-        <f>D17-($B$17/COUNTA($C$3:$K$3))</f>
+        <f t="shared" si="2"/>
         <v>8.6666666666666661</v>
       </c>
       <c r="F17" s="19">
-        <f>E17-($B$17/COUNTA($C$3:$K$3))</f>
+        <f t="shared" si="2"/>
         <v>7.2222222222222214</v>
       </c>
       <c r="G17" s="19">
-        <f>F17-($B$17/COUNTA($C$3:$K$3))</f>
+        <f t="shared" si="2"/>
         <v>5.7777777777777768</v>
       </c>
       <c r="H17" s="19">
-        <f>G17-($B$17/COUNTA($C$3:$K$3))</f>
+        <f t="shared" si="2"/>
         <v>4.3333333333333321</v>
       </c>
       <c r="I17" s="19">
-        <f>H17-($B$17/COUNTA($C$3:$K$3))</f>
+        <f t="shared" si="2"/>
         <v>2.8888888888888875</v>
       </c>
       <c r="J17" s="19">
-        <f t="shared" ref="J17:K17" si="1">I17-($B$17/COUNTA($C$3:$K$3))</f>
+        <f t="shared" ref="J17:K17" si="3">I17-($B$17/COUNTA($C$3:$K$3))</f>
         <v>1.4444444444444431</v>
       </c>
       <c r="K17" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L17" s="35">
@@ -17903,7 +19153,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.7109375" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="53" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="50" customWidth="1"/>
     <col min="3" max="15" width="9.85546875" customWidth="1"/>
     <col min="16" max="16" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.28515625" customWidth="1"/>
@@ -17911,27 +19161,27 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="40" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="66" t="s">
         <v>177</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="42"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="68"/>
     </row>
-    <row r="3" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="44"/>
-      <c r="B3" s="45" t="s">
+    <row r="3" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="41"/>
+      <c r="B3" s="42" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="21" t="s">
@@ -17978,7 +19228,7 @@
       <c r="A4" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="B4" s="54">
+      <c r="B4" s="51">
         <v>1</v>
       </c>
       <c r="C4" s="10"/>
@@ -17998,33 +19248,33 @@
       <c r="O4" s="11"/>
     </row>
     <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="49" t="s">
         <v>192</v>
       </c>
-      <c r="B5" s="55">
+      <c r="B5" s="52">
         <v>1</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49">
+      <c r="C5" s="46"/>
+      <c r="D5" s="46">
         <v>1.5</v>
       </c>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
-      <c r="O5" s="50"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="47"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="B6" s="56">
+      <c r="B6" s="53">
         <v>1</v>
       </c>
       <c r="C6" s="13"/>
@@ -18044,33 +19294,33 @@
       <c r="O6" s="14"/>
     </row>
     <row r="7" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="49" t="s">
         <v>194</v>
       </c>
-      <c r="B7" s="55">
+      <c r="B7" s="52">
         <v>3</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49">
+      <c r="C7" s="46"/>
+      <c r="D7" s="46">
         <v>4</v>
       </c>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="49"/>
-      <c r="O7" s="50"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="47"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="57">
+      <c r="B8" s="54">
         <f>SUM(B4:B7)</f>
         <v>6</v>
       </c>
@@ -18131,7 +19381,7 @@
       <c r="A9" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="58">
+      <c r="B9" s="55">
         <f>B8</f>
         <v>6</v>
       </c>
@@ -18221,7 +19471,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A2" sqref="A2:K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18230,23 +19480,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="53"/>
+      <c r="B1" s="50"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="40" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="66" t="s">
         <v>199</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="42"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="68"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="44"/>
-      <c r="B3" s="45" t="s">
+      <c r="A3" s="41"/>
+      <c r="B3" s="42" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="21" t="s">
@@ -18269,10 +19519,10 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="56" t="s">
         <v>196</v>
       </c>
-      <c r="B4" s="54">
+      <c r="B4" s="51">
         <v>1</v>
       </c>
       <c r="C4" s="10">
@@ -18285,26 +19535,26 @@
       <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="57" t="s">
         <v>195</v>
       </c>
-      <c r="B5" s="55">
+      <c r="B5" s="52">
         <v>0.5</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49">
+      <c r="C5" s="46"/>
+      <c r="D5" s="46">
         <v>0.75</v>
       </c>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="50"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="47"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="43" t="s">
         <v>197</v>
       </c>
-      <c r="B6" s="56">
+      <c r="B6" s="53">
         <v>0.75</v>
       </c>
       <c r="C6" s="13"/>
@@ -18317,26 +19567,26 @@
       <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="58" t="s">
         <v>198</v>
       </c>
-      <c r="B7" s="62">
+      <c r="B7" s="59">
         <v>1</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63">
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60">
         <v>4</v>
       </c>
-      <c r="G7" s="63"/>
-      <c r="H7" s="64"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="61"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="43" t="s">
         <v>206</v>
       </c>
-      <c r="B8" s="56">
+      <c r="B8" s="53">
         <v>2</v>
       </c>
       <c r="C8" s="13"/>
@@ -18349,26 +19599,26 @@
       <c r="H8" s="14"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="58" t="s">
         <v>207</v>
       </c>
-      <c r="B9" s="62">
+      <c r="B9" s="59">
         <v>3</v>
       </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63">
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60">
         <v>3</v>
       </c>
-      <c r="G9" s="63"/>
-      <c r="H9" s="64"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="61"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="43" t="s">
         <v>208</v>
       </c>
-      <c r="B10" s="56">
+      <c r="B10" s="53">
         <v>0.5</v>
       </c>
       <c r="C10" s="13"/>
@@ -18381,51 +19631,51 @@
       <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="57" t="s">
         <v>209</v>
       </c>
-      <c r="B11" s="55">
+      <c r="B11" s="52">
         <v>4</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49">
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46">
         <v>4</v>
       </c>
-      <c r="H11" s="50"/>
+      <c r="H11" s="47"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="57">
+      <c r="B12" s="54">
         <f>SUM(B4:B11)</f>
         <v>12.75</v>
       </c>
       <c r="C12" s="16">
-        <f>IF(B12-SUM(C4:C11)&gt;0,B12-SUM(C4:C11),0)</f>
+        <f t="shared" ref="C12:H12" si="0">IF(B12-SUM(C4:C11)&gt;0,B12-SUM(C4:C11),0)</f>
         <v>11.25</v>
       </c>
       <c r="D12" s="16">
-        <f>IF(C12-SUM(D4:D11)&gt;0,C12-SUM(D4:D11),0)</f>
+        <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
       <c r="E12" s="16">
-        <f>IF(D12-SUM(E4:E11)&gt;0,D12-SUM(E4:E11),0)</f>
+        <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
       <c r="F12" s="16">
-        <f>IF(E12-SUM(F4:F11)&gt;0,E12-SUM(F4:F11),0)</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="G12" s="16">
-        <f>IF(F12-SUM(G4:G11)&gt;0,F12-SUM(G4:G11),0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H12" s="17">
-        <f>IF(G12-SUM(H4:H11)&gt;0,G12-SUM(H4:H11),0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I12" s="34" t="s">
@@ -18439,32 +19689,32 @@
       <c r="A13" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="58">
+      <c r="B13" s="55">
         <f>B12</f>
         <v>12.75</v>
       </c>
       <c r="C13" s="19">
-        <f>B13-($B$13/COUNTA($C$3:$H$3))</f>
+        <f t="shared" ref="C13:H13" si="1">B13-($B$13/COUNTA($C$3:$H$3))</f>
         <v>10.625</v>
       </c>
       <c r="D13" s="19">
-        <f>C13-($B$13/COUNTA($C$3:$H$3))</f>
+        <f t="shared" si="1"/>
         <v>8.5</v>
       </c>
       <c r="E13" s="19">
-        <f>D13-($B$13/COUNTA($C$3:$H$3))</f>
+        <f t="shared" si="1"/>
         <v>6.375</v>
       </c>
       <c r="F13" s="19">
-        <f>E13-($B$13/COUNTA($C$3:$H$3))</f>
+        <f t="shared" si="1"/>
         <v>4.25</v>
       </c>
       <c r="G13" s="19">
-        <f>F13-($B$13/COUNTA($C$3:$H$3))</f>
+        <f t="shared" si="1"/>
         <v>2.125</v>
       </c>
       <c r="H13" s="20">
-        <f>G13-($B$13/COUNTA($C$3:$H$3))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I13" s="35">
@@ -18477,70 +19727,70 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="53"/>
+      <c r="B14" s="50"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="53"/>
+      <c r="B15" s="50"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="53"/>
+      <c r="B16" s="50"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="53"/>
+      <c r="B17" s="50"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="53"/>
+      <c r="B18" s="50"/>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="53"/>
+      <c r="B19" s="50"/>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="53"/>
+      <c r="B20" s="50"/>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="53"/>
+      <c r="B21" s="50"/>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="53"/>
+      <c r="B22" s="50"/>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="53"/>
+      <c r="B23" s="50"/>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="53"/>
+      <c r="B24" s="50"/>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="53"/>
+      <c r="B25" s="50"/>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="53"/>
+      <c r="B26" s="50"/>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="53"/>
+      <c r="B27" s="50"/>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="53"/>
+      <c r="B28" s="50"/>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="53"/>
+      <c r="B29" s="50"/>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="53"/>
+      <c r="B30" s="50"/>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="53"/>
+      <c r="B31" s="50"/>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="53"/>
+      <c r="B32" s="50"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="53"/>
+      <c r="B33" s="50"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="53"/>
+      <c r="B34" s="50"/>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="53"/>
+      <c r="B35" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -18553,10 +19803,333 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="70.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="44"/>
+      <c r="B2" s="66" t="s">
+        <v>219</v>
+      </c>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="68"/>
+    </row>
+    <row r="3" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="41"/>
+      <c r="B3" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="56" t="s">
+        <v>218</v>
+      </c>
+      <c r="B4" s="51">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="57" t="s">
+        <v>227</v>
+      </c>
+      <c r="B5" s="52">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46">
+        <v>0.75</v>
+      </c>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="47"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="43" t="s">
+        <v>228</v>
+      </c>
+      <c r="B6" s="53">
+        <v>12</v>
+      </c>
+      <c r="C6" s="13">
+        <v>5</v>
+      </c>
+      <c r="D6" s="13">
+        <v>5</v>
+      </c>
+      <c r="E6" s="13">
+        <v>5</v>
+      </c>
+      <c r="F6" s="13">
+        <v>5</v>
+      </c>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="14"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="58" t="s">
+        <v>229</v>
+      </c>
+      <c r="B7" s="59">
+        <v>0.25</v>
+      </c>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60">
+        <v>0.25</v>
+      </c>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="61"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
+        <v>231</v>
+      </c>
+      <c r="B8" s="53">
+        <v>10</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13">
+        <v>3</v>
+      </c>
+      <c r="G8" s="13">
+        <v>5</v>
+      </c>
+      <c r="H8" s="13">
+        <v>5</v>
+      </c>
+      <c r="I8" s="14"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="58" t="s">
+        <v>230</v>
+      </c>
+      <c r="B9" s="59">
+        <v>0.25</v>
+      </c>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60">
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="61"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="54">
+        <f>SUM(B4:B9)</f>
+        <v>23.5</v>
+      </c>
+      <c r="C10" s="16">
+        <f>IF(B10-SUM(C4:C9)&gt;0,B10-SUM(C4:C9),0)</f>
+        <v>18.5</v>
+      </c>
+      <c r="D10" s="16">
+        <f t="shared" ref="D10:I10" si="0">IF(C10-SUM(D4:D9)&gt;0,C10-SUM(D4:D9),0)</f>
+        <v>13.5</v>
+      </c>
+      <c r="E10" s="16">
+        <f t="shared" si="0"/>
+        <v>7.25</v>
+      </c>
+      <c r="F10" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="55">
+        <f>B10</f>
+        <v>23.5</v>
+      </c>
+      <c r="C11" s="19">
+        <f>B11-($B$11/COUNTA($C$3:$I$3))</f>
+        <v>20.142857142857142</v>
+      </c>
+      <c r="D11" s="19">
+        <f t="shared" ref="D11:I11" si="1">C11-($B$11/COUNTA($C$3:$I$3))</f>
+        <v>16.785714285714285</v>
+      </c>
+      <c r="E11" s="19">
+        <f t="shared" si="1"/>
+        <v>13.428571428571427</v>
+      </c>
+      <c r="F11" s="19">
+        <f t="shared" si="1"/>
+        <v>10.071428571428569</v>
+      </c>
+      <c r="G11" s="19">
+        <f t="shared" si="1"/>
+        <v>6.7142857142857117</v>
+      </c>
+      <c r="H11" s="19">
+        <f t="shared" si="1"/>
+        <v>3.3571428571428545</v>
+      </c>
+      <c r="I11" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="35">
+        <f>SUM(B4:B9)</f>
+        <v>23.5</v>
+      </c>
+      <c r="K11" s="35">
+        <f>SUM(C4:I9)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="50"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="50"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="50"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="50"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="50"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="50"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="50"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="50"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="50"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="50"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="50"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="50"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="50"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="50"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="50"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="50"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="50"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="50"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="50"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18585,16 +20158,16 @@
       <c r="A4" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="B4" s="66">
-        <v>19</v>
-      </c>
-      <c r="C4" s="65">
-        <f>SUM('Sprint 0'!C4:C10)+SUM('Sprint 1'!H8,'Sprint 1'!C3,'Sprint 1'!C4)+'Sprint 2'!I4+SUM('Sprint 8'!H6:H9,'Sprint 8'!G4:G5)+'Sprint 9'!G14+'Sprint 11'!$C$4</f>
-        <v>10.700001</v>
-      </c>
-      <c r="E4" s="67">
+      <c r="B4" s="63">
+        <v>24</v>
+      </c>
+      <c r="C4" s="62">
+        <f>SUM('Sprint 0'!C4:C10)+SUM('Sprint 1'!H8,'Sprint 1'!C3,'Sprint 1'!C4)+'Sprint 2'!I4+SUM('Sprint 8'!H6:H9,'Sprint 8'!G4:G5)+'Sprint 9'!G14+'Sprint 11'!$C$4+SUM('Sprint 12'!$E$4:$E$5,'Sprint 12'!$C$6:$F$6,'Sprint 12'!$F$7,'Sprint 12'!$F$8:$H$8)</f>
+        <v>45.200001</v>
+      </c>
+      <c r="E4" s="64">
         <f>C4/$C$9</f>
-        <v>6.8174583828132643E-2</v>
+        <v>0.23547799304257364</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -18604,13 +20177,13 @@
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5" s="65">
+      <c r="C5" s="62">
         <f>'Sprint 9'!G13+SUM('Sprint 11'!$F$9,'Sprint 11'!$F$8)</f>
         <v>7</v>
       </c>
-      <c r="E5" s="67">
+      <c r="E5" s="64">
         <f t="shared" ref="E5:E7" si="0">C5/$C$9</f>
-        <v>4.4600190859508185E-2</v>
+        <v>3.6467829974119147E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -18618,15 +20191,15 @@
         <v>212</v>
       </c>
       <c r="B6">
-        <v>12</v>
-      </c>
-      <c r="C6" s="65">
-        <f>'Sprint 1'!I9+'Sprint 8'!I11+SUM('Sprint 9'!D4,'Sprint 9'!D5,'Sprint 9'!E9,'Sprint 9'!E10,'Sprint 9'!G12)+SUM('Sprint 11'!$F$8,'Sprint 11'!$D$5)</f>
-        <v>15.25</v>
-      </c>
-      <c r="E6" s="67">
+        <v>13</v>
+      </c>
+      <c r="C6" s="62">
+        <f>'Sprint 1'!I9+'Sprint 8'!I11+SUM('Sprint 9'!D4,'Sprint 9'!D5,'Sprint 9'!E9,'Sprint 9'!E10,'Sprint 9'!G12)+SUM('Sprint 11'!$F$8,'Sprint 11'!$D$5)+'Sprint 12'!$H$9</f>
+        <v>15.75</v>
+      </c>
+      <c r="E6" s="64">
         <f t="shared" si="0"/>
-        <v>9.7164701515357124E-2</v>
+        <v>8.2052617441768089E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -18636,23 +20209,23 @@
       <c r="B7">
         <v>63</v>
       </c>
-      <c r="C7" s="65">
+      <c r="C7" s="62">
         <f>SUM('Sprint 1'!F5,'Sprint 1'!I9,'Sprint 1'!I12,'Sprint 1'!I11,'Sprint 1'!I10,'Sprint 1'!F7,'Sprint 1'!F6)+SUM('Sprint 2'!I5:I8)+SUM('Sprint 3'!E4:E5,'Sprint 3'!F6:F7,'Sprint 3'!H8:H10)+SUM('Sprint 4'!H4:H6)+SUM('Sprint 5'!H4:H5)+SUM('Sprint 6'!R4:R9)+SUM('Sprint 7'!K4:K6,'Sprint 7'!O8:O10,'Sprint 7'!P11:P14)+SUM('Sprint 8'!J12,'Sprint 8'!I10,'Sprint 8'!G5)+SUM('Sprint 9'!K15,'Sprint 9'!E11,'Sprint 9'!E9,'Sprint 9'!E8,'Sprint 9'!D7,'Sprint 9'!D6)+SUM('Sprint 10'!D4:D7)+SUM('Sprint 11'!$G$11,'Sprint 11'!$G$10,'Sprint 11'!$F$7,'Sprint 11'!$D$6)</f>
         <v>124</v>
       </c>
-      <c r="E7" s="67">
+      <c r="E7" s="64">
         <f t="shared" si="0"/>
-        <v>0.7900605237970022</v>
+        <v>0.64600155954153915</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="68">
+      <c r="B9" s="65">
         <f>SUM(B4:B7)</f>
-        <v>97</v>
-      </c>
-      <c r="C9" s="65">
+        <v>103</v>
+      </c>
+      <c r="C9" s="62">
         <f>SUM(C4:C7)</f>
-        <v>156.95000099999999</v>
+        <v>191.95000099999999</v>
       </c>
     </row>
   </sheetData>
@@ -18679,16 +20252,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="42"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="68"/>
       <c r="M1" s="1">
         <v>0.25</v>
       </c>
@@ -19042,16 +20615,16 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="42"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="68"/>
       <c r="M2" s="1">
         <v>0.25</v>
       </c>
@@ -19320,16 +20893,16 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="42"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="68"/>
       <c r="M2" s="1">
         <v>0.25</v>
       </c>
@@ -19620,16 +21193,16 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="42"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="68"/>
     </row>
     <row r="3" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -19820,16 +21393,16 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="42"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="68"/>
     </row>
     <row r="3" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -20005,25 +21578,25 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="42"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="68"/>
     </row>
     <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -20424,28 +21997,28 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="43"/>
-      <c r="B2" s="40" t="s">
+      <c r="A2" s="40"/>
+      <c r="B2" s="66" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="42"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="68"/>
     </row>
-    <row r="3" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="44"/>
-      <c r="B3" s="45" t="s">
+    <row r="3" spans="1:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="41"/>
+      <c r="B3" s="42" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="21" t="s">
@@ -20564,7 +22137,7 @@
       <c r="P6" s="14"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="43" t="s">
         <v>129</v>
       </c>
       <c r="B7" s="13">
@@ -20764,59 +22337,59 @@
         <v>16.75</v>
       </c>
       <c r="C15" s="16">
-        <f>IF(B15-SUM(C4:C14)&gt;0,B15-SUM(C4:C14),0)</f>
+        <f t="shared" ref="C15:P15" si="0">IF(B15-SUM(C4:C14)&gt;0,B15-SUM(C4:C14),0)</f>
         <v>16.75</v>
       </c>
       <c r="D15" s="16">
-        <f>IF(C15-SUM(D4:D14)&gt;0,C15-SUM(D4:D14),0)</f>
+        <f t="shared" si="0"/>
         <v>16.75</v>
       </c>
       <c r="E15" s="16">
-        <f>IF(D15-SUM(E4:E14)&gt;0,D15-SUM(E4:E14),0)</f>
+        <f t="shared" si="0"/>
         <v>16.75</v>
       </c>
       <c r="F15" s="16">
-        <f>IF(E15-SUM(F4:F14)&gt;0,E15-SUM(F4:F14),0)</f>
+        <f t="shared" si="0"/>
         <v>16.75</v>
       </c>
       <c r="G15" s="16">
-        <f>IF(F15-SUM(G4:G14)&gt;0,F15-SUM(G4:G14),0)</f>
+        <f t="shared" si="0"/>
         <v>16.75</v>
       </c>
       <c r="H15" s="16">
-        <f>IF(G15-SUM(H4:H14)&gt;0,G15-SUM(H4:H14),0)</f>
+        <f t="shared" si="0"/>
         <v>16.75</v>
       </c>
       <c r="I15" s="16">
-        <f>IF(H15-SUM(I4:I14)&gt;0,H15-SUM(I4:I14),0)</f>
+        <f t="shared" si="0"/>
         <v>16.75</v>
       </c>
       <c r="J15" s="16">
-        <f>IF(I15-SUM(J4:J14)&gt;0,I15-SUM(J4:J14),0)</f>
+        <f t="shared" si="0"/>
         <v>16.75</v>
       </c>
       <c r="K15" s="16">
-        <f>IF(J15-SUM(K4:K14)&gt;0,J15-SUM(K4:K14),0)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L15" s="16">
-        <f>IF(K15-SUM(L4:L14)&gt;0,K15-SUM(L4:L14),0)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="M15" s="16">
-        <f>IF(L15-SUM(M4:M14)&gt;0,L15-SUM(M4:M14),0)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="N15" s="16">
-        <f>IF(M15-SUM(N4:N14)&gt;0,M15-SUM(N4:N14),0)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="O15" s="16">
-        <f>IF(N15-SUM(O4:O14)&gt;0,N15-SUM(O4:O14),0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P15" s="17">
-        <f>IF(O15-SUM(P4:P14)&gt;0,O15-SUM(P4:P14),0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -20829,59 +22402,59 @@
         <v>16.75</v>
       </c>
       <c r="C16" s="19">
-        <f>B16-($B$16/COUNTA($C$3:$P$3))</f>
+        <f t="shared" ref="C16:P16" si="1">B16-($B$16/COUNTA($C$3:$P$3))</f>
         <v>15.553571428571429</v>
       </c>
       <c r="D16" s="19">
-        <f>C16-($B$16/COUNTA($C$3:$P$3))</f>
+        <f t="shared" si="1"/>
         <v>14.357142857142858</v>
       </c>
       <c r="E16" s="19">
-        <f>D16-($B$16/COUNTA($C$3:$P$3))</f>
+        <f t="shared" si="1"/>
         <v>13.160714285714286</v>
       </c>
       <c r="F16" s="19">
-        <f>E16-($B$16/COUNTA($C$3:$P$3))</f>
+        <f t="shared" si="1"/>
         <v>11.964285714285715</v>
       </c>
       <c r="G16" s="19">
-        <f>F16-($B$16/COUNTA($C$3:$P$3))</f>
+        <f t="shared" si="1"/>
         <v>10.767857142857144</v>
       </c>
       <c r="H16" s="19">
-        <f>G16-($B$16/COUNTA($C$3:$P$3))</f>
+        <f t="shared" si="1"/>
         <v>9.571428571428573</v>
       </c>
       <c r="I16" s="19">
-        <f>H16-($B$16/COUNTA($C$3:$P$3))</f>
+        <f t="shared" si="1"/>
         <v>8.3750000000000018</v>
       </c>
       <c r="J16" s="19">
-        <f>I16-($B$16/COUNTA($C$3:$P$3))</f>
+        <f t="shared" si="1"/>
         <v>7.1785714285714306</v>
       </c>
       <c r="K16" s="19">
-        <f>J16-($B$16/COUNTA($C$3:$P$3))</f>
+        <f t="shared" si="1"/>
         <v>5.9821428571428594</v>
       </c>
       <c r="L16" s="19">
-        <f>K16-($B$16/COUNTA($C$3:$P$3))</f>
+        <f t="shared" si="1"/>
         <v>4.7857142857142883</v>
       </c>
       <c r="M16" s="19">
-        <f>L16-($B$16/COUNTA($C$3:$P$3))</f>
+        <f t="shared" si="1"/>
         <v>3.5892857142857171</v>
       </c>
       <c r="N16" s="19">
-        <f>M16-($B$16/COUNTA($C$3:$P$3))</f>
+        <f t="shared" si="1"/>
         <v>2.3928571428571459</v>
       </c>
       <c r="O16" s="19">
-        <f>N16-($B$16/COUNTA($C$3:$P$3))</f>
+        <f t="shared" si="1"/>
         <v>1.1964285714285745</v>
       </c>
       <c r="P16" s="20">
-        <f>O16-($B$16/COUNTA($C$3:$P$3))</f>
+        <f t="shared" si="1"/>
         <v>3.1086244689504383E-15</v>
       </c>
     </row>
@@ -20927,22 +22500,22 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="40" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="66" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="68"/>
     </row>
     <row r="3" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="44"/>
-      <c r="B3" s="45" t="s">
+      <c r="A3" s="41"/>
+      <c r="B3" s="42" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="21" t="s">
@@ -21025,7 +22598,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="43" t="s">
         <v>149</v>
       </c>
       <c r="B7" s="13">
@@ -21141,35 +22714,35 @@
         <v>6.25</v>
       </c>
       <c r="C13" s="16">
-        <f>IF(B13-SUM(C4:C12)&gt;0,B13-SUM(C4:C12),0)</f>
+        <f t="shared" ref="C13:J13" si="0">IF(B13-SUM(C4:C12)&gt;0,B13-SUM(C4:C12),0)</f>
         <v>6.25</v>
       </c>
       <c r="D13" s="16">
-        <f>IF(C13-SUM(D4:D12)&gt;0,C13-SUM(D4:D12),0)</f>
+        <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
       <c r="E13" s="16">
-        <f>IF(D13-SUM(E4:E12)&gt;0,D13-SUM(E4:E12),0)</f>
+        <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
       <c r="F13" s="16">
-        <f>IF(E13-SUM(F4:F12)&gt;0,E13-SUM(F4:F12),0)</f>
+        <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
       <c r="G13" s="16">
-        <f>IF(F13-SUM(G4:G12)&gt;0,F13-SUM(G4:G12),0)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H13" s="16">
-        <f>IF(G13-SUM(H4:H12)&gt;0,G13-SUM(H4:H12),0)</f>
+        <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
       <c r="I13" s="16">
-        <f>IF(H13-SUM(I4:I12)&gt;0,H13-SUM(I4:I12),0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J13" s="17">
-        <f>IF(I13-SUM(J4:J12)&gt;0,I13-SUM(J4:J12),0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K13" s="34" t="s">
@@ -21188,35 +22761,35 @@
         <v>6.25</v>
       </c>
       <c r="C14" s="19">
-        <f>B14-($B$14/COUNTA($C$3:$J$3))</f>
+        <f t="shared" ref="C14:J14" si="1">B14-($B$14/COUNTA($C$3:$J$3))</f>
         <v>5.46875</v>
       </c>
       <c r="D14" s="19">
-        <f>C14-($B$14/COUNTA($C$3:$J$3))</f>
+        <f t="shared" si="1"/>
         <v>4.6875</v>
       </c>
       <c r="E14" s="19">
-        <f>D14-($B$14/COUNTA($C$3:$J$3))</f>
+        <f t="shared" si="1"/>
         <v>3.90625</v>
       </c>
       <c r="F14" s="19">
-        <f>E14-($B$14/COUNTA($C$3:$J$3))</f>
+        <f t="shared" si="1"/>
         <v>3.125</v>
       </c>
       <c r="G14" s="19">
-        <f>F14-($B$14/COUNTA($C$3:$J$3))</f>
+        <f t="shared" si="1"/>
         <v>2.34375</v>
       </c>
       <c r="H14" s="19">
-        <f>G14-($B$14/COUNTA($C$3:$J$3))</f>
+        <f t="shared" si="1"/>
         <v>1.5625</v>
       </c>
       <c r="I14" s="19">
-        <f>H14-($B$14/COUNTA($C$3:$J$3))</f>
+        <f t="shared" si="1"/>
         <v>0.78125</v>
       </c>
       <c r="J14" s="20">
-        <f>I14-($B$14/COUNTA($C$3:$J$3))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K14" s="35">

</xml_diff>

<commit_message>
Documentado el tercer anexo (Especificación de diseño).
</commit_message>
<xml_diff>
--- a/doc/latex/Scrum.xlsx
+++ b/doc/latex/Scrum.xlsx
@@ -25,7 +25,8 @@
     <sheet name="Sprint 10" sheetId="12" r:id="rId11"/>
     <sheet name="Sprint 11" sheetId="13" r:id="rId12"/>
     <sheet name="Sprint 12" sheetId="15" r:id="rId13"/>
-    <sheet name="Resumen" sheetId="14" r:id="rId14"/>
+    <sheet name="Sprint 13" sheetId="16" r:id="rId14"/>
+    <sheet name="Resumen" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="239">
   <si>
     <t>Elegir el lenguaje de programación</t>
   </si>
@@ -717,9 +718,6 @@
     <t>Día 6 (13/06/17)</t>
   </si>
   <si>
-    <t>Día 7 (14/06/17)</t>
-  </si>
-  <si>
     <t>Añadir documento de licencia GNU GPL.</t>
   </si>
   <si>
@@ -733,6 +731,30 @@
   </si>
   <si>
     <t>Documentar el segundo anexo (especificación de requisitos).</t>
+  </si>
+  <si>
+    <t>Añadir páginas de error propias.</t>
+  </si>
+  <si>
+    <t>Sprint 13 (14/06/17 - 19/06/17)</t>
+  </si>
+  <si>
+    <t>Día 1 (14/06/17)</t>
+  </si>
+  <si>
+    <t>Día 2 (15/06/17)</t>
+  </si>
+  <si>
+    <t>Día 3 (16/06/17)</t>
+  </si>
+  <si>
+    <t>Día 4 (17/06/17)</t>
+  </si>
+  <si>
+    <t>Día 5 (18/06/17)</t>
+  </si>
+  <si>
+    <t>Día 6 (19/06/17)</t>
   </si>
 </sst>
 </file>
@@ -3601,9 +3623,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 12'!$B$3:$I$3</c:f>
+              <c:f>'Sprint 12'!$B$3:$H$3</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Total Horas</c:v>
                 </c:pt>
@@ -3624,19 +3646,16 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Día 6 (13/06/17)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Día 7 (14/06/17)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 12'!$B$10:$I$10</c:f>
+              <c:f>'Sprint 12'!$B$10:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>23.5</c:v>
                 </c:pt>
@@ -3656,9 +3675,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3699,9 +3715,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 12'!$B$3:$I$3</c:f>
+              <c:f>'Sprint 12'!$B$3:$H$3</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Total Horas</c:v>
                 </c:pt>
@@ -3722,41 +3738,35 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Día 6 (13/06/17)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Día 7 (14/06/17)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 12'!$B$11:$I$11</c:f>
+              <c:f>'Sprint 12'!$B$11:$H$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>23.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.142857142857142</c:v>
+                  <c:v>19.583333333333332</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.785714285714285</c:v>
+                  <c:v>15.666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.428571428571427</c:v>
+                  <c:v>11.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.071428571428569</c:v>
+                  <c:v>7.8333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.7142857142857117</c:v>
+                  <c:v>3.9166666666666674</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3571428571428545</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4076,6 +4086,571 @@
 </file>
 
 <file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>Sprint 13</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 13'!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Restante</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 13'!$B$3:$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Total Horas</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Día 1 (14/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Día 2 (15/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Día 3 (16/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Día 4 (17/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Día 5 (18/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Día 6 (19/06/17)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 13'!$B$10:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FC72-45F2-AA2D-090A1DF50032}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 13'!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 13'!$B$3:$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Total Horas</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Día 1 (14/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Día 2 (15/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Día 3 (16/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Día 4 (17/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Día 5 (18/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Día 6 (19/06/17)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 13'!$B$11:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.41666666666666669</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33333333333333337</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25000000000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16666666666666674</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.3333333333333412E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FC72-45F2-AA2D-090A1DF50032}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="404108848"/>
+        <c:axId val="404106880"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="404108848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Dias</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="404106880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="404106880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Horas</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="404108848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -9511,6 +10086,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -12347,6 +12962,509 @@
 </file>
 
 <file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="258">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -17275,23 +18393,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>372364</xdr:colOff>
+      <xdr:colOff>524764</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>151530</xdr:rowOff>
+      <xdr:rowOff>103905</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8E0048D-02F5-48A2-A201-4E77346ED138}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B578008-1CDC-419B-980A-680E9D8CF353}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17307,7 +18425,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6086475" y="2752725"/>
+          <a:off x="6238875" y="2705100"/>
           <a:ext cx="5858764" cy="3151905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -17321,6 +18439,49 @@
 </file>
 
 <file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19053</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{957F500A-C2A7-4A3E-99A2-DC694157DC89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -19803,10 +20964,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection sqref="A1:K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19814,8 +20975,8 @@
     <col min="1" max="1" width="70.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
       <c r="B2" s="66" t="s">
         <v>219</v>
@@ -19826,9 +20987,8 @@
       <c r="F2" s="67"/>
       <c r="G2" s="67"/>
       <c r="H2" s="67"/>
-      <c r="I2" s="68"/>
     </row>
-    <row r="3" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="42" t="s">
         <v>7</v>
@@ -19851,11 +21011,8 @@
       <c r="H3" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="I3" s="22" t="s">
-        <v>226</v>
-      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
         <v>218</v>
       </c>
@@ -19870,11 +21027,10 @@
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
-      <c r="I4" s="11"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B5" s="52">
         <v>0.5</v>
@@ -19887,11 +21043,10 @@
       <c r="F5" s="46"/>
       <c r="G5" s="46"/>
       <c r="H5" s="46"/>
-      <c r="I5" s="47"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B6" s="53">
         <v>12</v>
@@ -19910,11 +21065,10 @@
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
-      <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B7" s="59">
         <v>0.25</v>
@@ -19927,11 +21081,10 @@
       </c>
       <c r="G7" s="60"/>
       <c r="H7" s="60"/>
-      <c r="I7" s="61"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B8" s="53">
         <v>10</v>
@@ -19948,11 +21101,10 @@
       <c r="H8" s="13">
         <v>5</v>
       </c>
-      <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="58" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B9" s="59">
         <v>0.25</v>
@@ -19965,9 +21117,8 @@
       <c r="H9" s="60">
         <v>0.5</v>
       </c>
-      <c r="I9" s="61"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>12</v>
       </c>
@@ -19980,7 +21131,7 @@
         <v>18.5</v>
       </c>
       <c r="D10" s="16">
-        <f t="shared" ref="D10:I10" si="0">IF(C10-SUM(D4:D9)&gt;0,C10-SUM(D4:D9),0)</f>
+        <f t="shared" ref="D10:H10" si="0">IF(C10-SUM(D4:D9)&gt;0,C10-SUM(D4:D9),0)</f>
         <v>13.5</v>
       </c>
       <c r="E10" s="16">
@@ -19999,18 +21150,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I10" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="I10" s="34" t="s">
+        <v>13</v>
       </c>
       <c r="J10" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="K10" s="34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>13</v>
       </c>
@@ -20019,55 +21166,51 @@
         <v>23.5</v>
       </c>
       <c r="C11" s="19">
-        <f>B11-($B$11/COUNTA($C$3:$I$3))</f>
-        <v>20.142857142857142</v>
+        <f t="shared" ref="C11:H11" si="1">B11-($B$11/COUNTA($C$3:$H$3))</f>
+        <v>19.583333333333332</v>
       </c>
       <c r="D11" s="19">
-        <f t="shared" ref="D11:I11" si="1">C11-($B$11/COUNTA($C$3:$I$3))</f>
-        <v>16.785714285714285</v>
+        <f t="shared" si="1"/>
+        <v>15.666666666666666</v>
       </c>
       <c r="E11" s="19">
         <f t="shared" si="1"/>
-        <v>13.428571428571427</v>
+        <v>11.75</v>
       </c>
       <c r="F11" s="19">
         <f t="shared" si="1"/>
-        <v>10.071428571428569</v>
+        <v>7.8333333333333339</v>
       </c>
       <c r="G11" s="19">
         <f t="shared" si="1"/>
-        <v>6.7142857142857117</v>
+        <v>3.9166666666666674</v>
       </c>
       <c r="H11" s="19">
         <f t="shared" si="1"/>
-        <v>3.3571428571428545</v>
-      </c>
-      <c r="I11" s="19">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J11" s="35">
+      <c r="I11" s="35">
         <f>SUM(B4:B9)</f>
         <v>23.5</v>
       </c>
-      <c r="K11" s="35">
-        <f>SUM(C4:I9)</f>
+      <c r="J11" s="35">
+        <f>SUM(C4:H9)</f>
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="50"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="50"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="50"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="50"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="50"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
@@ -20117,7 +21260,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -20126,9 +21269,274 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="44"/>
+      <c r="B2" s="66" t="s">
+        <v>232</v>
+      </c>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="68"/>
+    </row>
+    <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="41"/>
+      <c r="B3" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="56" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4" s="51">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="10">
+        <v>1</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="57"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="47"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="43"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="58"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="61"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="43"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="58"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="61"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="54">
+        <f>SUM(B4:B9)</f>
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="16">
+        <f>IF(B10-SUM(C4:C9)&gt;0,B10-SUM(C4:C9),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="16">
+        <f t="shared" ref="D10:H10" si="0">IF(C10-SUM(D4:D9)&gt;0,C10-SUM(D4:D9),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="55">
+        <f>B10</f>
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="19">
+        <f t="shared" ref="C11:H11" si="1">B11-($B$11/COUNTA($C$3:$H$3))</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D11" s="19">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="E11" s="19">
+        <f t="shared" si="1"/>
+        <v>0.25000000000000006</v>
+      </c>
+      <c r="F11" s="19">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666674</v>
+      </c>
+      <c r="G11" s="19">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333412E-2</v>
+      </c>
+      <c r="H11" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="35">
+        <f>SUM(B4:B9)</f>
+        <v>0.5</v>
+      </c>
+      <c r="J11" s="35">
+        <f>SUM(C4:H9)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="50"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="50"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="50"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="50"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="50"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="50"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="50"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="50"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="50"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="50"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="50"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="50"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="50"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="50"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="50"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="50"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="50"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="50"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="50"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Documentado el cuarto anexo (Documentación técnica de programación) y añadidos pequeños cambios a la memoria.
</commit_message>
<xml_diff>
--- a/doc/latex/Scrum.xlsx
+++ b/doc/latex/Scrum.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="241">
   <si>
     <t>Elegir el lenguaje de programación</t>
   </si>
@@ -756,6 +756,12 @@
   <si>
     <t>Día 6 (19/06/17)</t>
   </si>
+  <si>
+    <t>Documentar el tercer anexo (Especificación de diseño).</t>
+  </si>
+  <si>
+    <t>Documentar el cuarto anexo (Documentación técnica de programación).</t>
+  </si>
 </sst>
 </file>
 
@@ -991,7 +997,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
@@ -1105,6 +1111,10 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Énfasis3" xfId="5" builtinId="38"/>
@@ -4222,19 +4232,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -4314,22 +4324,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41666666666666669</c:v>
+                  <c:v>10.416666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.33333333333333337</c:v>
+                  <c:v>8.3333333333333321</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25000000000000006</c:v>
+                  <c:v>6.2499999999999982</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.16666666666666674</c:v>
+                  <c:v>4.1666666666666643</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.3333333333333412E-2</c:v>
+                  <c:v>2.0833333333333308</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -21271,13 +21281,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -21334,9 +21344,15 @@
       <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="57"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="46"/>
+      <c r="A5" s="57" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" s="69">
+        <v>5</v>
+      </c>
+      <c r="C5" s="70">
+        <v>7</v>
+      </c>
       <c r="D5" s="46"/>
       <c r="E5" s="46"/>
       <c r="F5" s="46"/>
@@ -21344,13 +21360,23 @@
       <c r="H5" s="47"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
-      <c r="B6" s="53"/>
+      <c r="A6" s="43" t="s">
+        <v>240</v>
+      </c>
+      <c r="B6" s="53">
+        <v>7</v>
+      </c>
       <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="D6" s="13">
+        <v>2</v>
+      </c>
       <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
+      <c r="F6" s="13">
+        <v>2</v>
+      </c>
+      <c r="G6" s="13">
+        <v>3</v>
+      </c>
       <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -21389,23 +21415,23 @@
       </c>
       <c r="B10" s="54">
         <f>SUM(B4:B9)</f>
-        <v>0.5</v>
+        <v>12.5</v>
       </c>
       <c r="C10" s="16">
         <f>IF(B10-SUM(C4:C9)&gt;0,B10-SUM(C4:C9),0)</f>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="D10" s="16">
         <f t="shared" ref="D10:H10" si="0">IF(C10-SUM(D4:D9)&gt;0,C10-SUM(D4:D9),0)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="E10" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="F10" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G10" s="16">
         <f t="shared" si="0"/>
@@ -21428,27 +21454,27 @@
       </c>
       <c r="B11" s="55">
         <f>B10</f>
-        <v>0.5</v>
+        <v>12.5</v>
       </c>
       <c r="C11" s="19">
         <f t="shared" ref="C11:H11" si="1">B11-($B$11/COUNTA($C$3:$H$3))</f>
-        <v>0.41666666666666669</v>
+        <v>10.416666666666666</v>
       </c>
       <c r="D11" s="19">
         <f t="shared" si="1"/>
-        <v>0.33333333333333337</v>
+        <v>8.3333333333333321</v>
       </c>
       <c r="E11" s="19">
         <f t="shared" si="1"/>
-        <v>0.25000000000000006</v>
+        <v>6.2499999999999982</v>
       </c>
       <c r="F11" s="19">
         <f t="shared" si="1"/>
-        <v>0.16666666666666674</v>
+        <v>4.1666666666666643</v>
       </c>
       <c r="G11" s="19">
         <f t="shared" si="1"/>
-        <v>8.3333333333333412E-2</v>
+        <v>2.0833333333333308</v>
       </c>
       <c r="H11" s="20">
         <f t="shared" si="1"/>
@@ -21456,11 +21482,11 @@
       </c>
       <c r="I11" s="35">
         <f>SUM(B4:B9)</f>
-        <v>0.5</v>
+        <v>12.5</v>
       </c>
       <c r="J11" s="35">
         <f>SUM(C4:H9)</f>
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Documentado el quinto anexo (Documentación de usuario).
</commit_message>
<xml_diff>
--- a/doc/latex/Scrum.xlsx
+++ b/doc/latex/Scrum.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16215" windowHeight="7530" firstSheet="6" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16215" windowHeight="7530" firstSheet="7" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 0" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="245">
   <si>
     <t>Elegir el lenguaje de programación</t>
   </si>
@@ -688,9 +688,6 @@
     <t>Horas</t>
   </si>
   <si>
-    <t>Hasta Sprint 11</t>
-  </si>
-  <si>
     <t>Porcentaje</t>
   </si>
   <si>
@@ -761,6 +758,21 @@
   </si>
   <si>
     <t>Documentar el cuarto anexo (Documentación técnica de programación).</t>
+  </si>
+  <si>
+    <t>Documentar el quinto anexo (Documentación de usuario).</t>
+  </si>
+  <si>
+    <t>Eliminar bugs encontrados por SonarQube.</t>
+  </si>
+  <si>
+    <t>Hasta Sprint 13</t>
+  </si>
+  <si>
+    <t>Añadir test unitario ausente de la clase DatabaseAdministration.</t>
+  </si>
+  <si>
+    <t>Añadir SonarQube como herramienta de medición de calidad de código.</t>
   </si>
 </sst>
 </file>
@@ -805,7 +817,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -853,6 +865,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -997,7 +1015,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
@@ -1099,9 +1117,18 @@
     <xf numFmtId="2" fontId="1" fillId="9" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="9" borderId="10" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="1" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="7" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="1" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="10" borderId="10" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1111,10 +1138,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Énfasis3" xfId="5" builtinId="38"/>
@@ -4175,7 +4198,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 13'!$A$10</c:f>
+              <c:f>'Sprint 13'!$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4227,24 +4250,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 13'!$B$10:$H$10</c:f>
+              <c:f>'Sprint 13'!$B$11:$H$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>12.5</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5</c:v>
+                  <c:v>4.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -4267,7 +4290,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 13'!$A$11</c:f>
+              <c:f>'Sprint 13'!$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4319,27 +4342,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 13'!$B$11:$H$11</c:f>
+              <c:f>'Sprint 13'!$B$12:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>12.5</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.416666666666666</c:v>
+                  <c:v>13.333333333333334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.3333333333333321</c:v>
+                  <c:v>10.666666666666668</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.2499999999999982</c:v>
+                  <c:v>8.0000000000000018</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1666666666666643</c:v>
+                  <c:v>5.3333333333333357</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0833333333333308</c:v>
+                  <c:v>2.6666666666666692</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -4929,16 +4952,16 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.23547799304257364</c:v>
+                  <c:v>0.29678328576293361</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.6467829974119147E-2</c:v>
+                  <c:v>3.7567503932531096E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.2052617441768089E-2</c:v>
+                  <c:v>7.8656961358736982E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.64600155954153915</c:v>
+                  <c:v>0.58699224894579838</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18454,13 +18477,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>19053</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -18486,6 +18509,50 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>126208</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>132480</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45FDA65E-37EF-453F-AEBC-4F30CECB74D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5838825" y="2924175"/>
+          <a:ext cx="5517358" cy="3151905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -18544,10 +18611,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98A57A69-B128-4DE9-A777-101AE63D61BD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41E8B1F2-9153-42B3-890B-D7130CB26EBD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19586,16 +19653,16 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="68"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="73"/>
       <c r="L2" s="3">
         <v>1</v>
       </c>
@@ -19926,18 +19993,18 @@
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="71" t="s">
         <v>175</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="68"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="73"/>
     </row>
     <row r="3" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
@@ -20333,22 +20400,22 @@
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="71" t="s">
         <v>177</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="68"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="73"/>
     </row>
     <row r="3" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
@@ -20655,15 +20722,15 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="71" t="s">
         <v>199</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="68"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="73"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
@@ -20988,15 +21055,15 @@
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
-      <c r="B2" s="66" t="s">
-        <v>219</v>
-      </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
+      <c r="B2" s="71" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
@@ -21004,27 +21071,27 @@
         <v>7</v>
       </c>
       <c r="C3" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="E3" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="F3" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="G3" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="H3" s="21" t="s">
         <v>224</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B4" s="51">
         <v>0.5</v>
@@ -21040,7 +21107,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B5" s="52">
         <v>0.5</v>
@@ -21056,7 +21123,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B6" s="53">
         <v>12</v>
@@ -21078,7 +21145,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B7" s="59">
         <v>0.25</v>
@@ -21094,7 +21161,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B8" s="53">
         <v>10</v>
@@ -21114,7 +21181,7 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="58" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B9" s="59">
         <v>0.25</v>
@@ -21279,10 +21346,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21293,15 +21360,15 @@
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
-      <c r="B2" s="66" t="s">
-        <v>232</v>
-      </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="68"/>
+      <c r="B2" s="71" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="73"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
@@ -21309,27 +21376,27 @@
         <v>7</v>
       </c>
       <c r="C3" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="E3" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="F3" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="G3" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="H3" s="22" t="s">
         <v>237</v>
-      </c>
-      <c r="H3" s="22" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B4" s="51">
         <v>0.5</v>
@@ -21345,12 +21412,12 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
-        <v>239</v>
-      </c>
-      <c r="B5" s="69">
+        <v>238</v>
+      </c>
+      <c r="B5" s="65">
         <v>5</v>
       </c>
-      <c r="C5" s="70">
+      <c r="C5" s="66">
         <v>7</v>
       </c>
       <c r="D5" s="46"/>
@@ -21361,7 +21428,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B6" s="53">
         <v>7</v>
@@ -21370,127 +21437,160 @@
       <c r="D6" s="13">
         <v>2</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13">
-        <v>2</v>
-      </c>
-      <c r="G6" s="13">
-        <v>3</v>
-      </c>
+      <c r="E6" s="13">
+        <v>5</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
       <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="58"/>
-      <c r="B7" s="59"/>
+      <c r="A7" s="58" t="s">
+        <v>243</v>
+      </c>
+      <c r="B7" s="59">
+        <v>0.5</v>
+      </c>
       <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
+      <c r="D7" s="60">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="60">
+        <v>0.5</v>
+      </c>
       <c r="F7" s="60"/>
       <c r="G7" s="60"/>
       <c r="H7" s="61"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="14"/>
+      <c r="A8" s="67" t="s">
+        <v>244</v>
+      </c>
+      <c r="B8" s="68">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69">
+        <v>0.75</v>
+      </c>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="70"/>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="58"/>
-      <c r="B9" s="59"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="58" t="s">
+        <v>241</v>
+      </c>
+      <c r="B9" s="59">
+        <v>0.5</v>
+      </c>
       <c r="C9" s="60"/>
       <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
+      <c r="E9" s="60">
+        <v>1</v>
+      </c>
       <c r="F9" s="60"/>
       <c r="G9" s="60"/>
       <c r="H9" s="61"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="43" t="s">
+        <v>240</v>
+      </c>
+      <c r="B10" s="53">
+        <v>2</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13">
+        <v>1</v>
+      </c>
+      <c r="G10" s="13">
+        <v>3</v>
+      </c>
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="54">
-        <f>SUM(B4:B9)</f>
-        <v>12.5</v>
-      </c>
-      <c r="C10" s="16">
-        <f>IF(B10-SUM(C4:C9)&gt;0,B10-SUM(C4:C9),0)</f>
-        <v>4.5</v>
-      </c>
-      <c r="D10" s="16">
-        <f t="shared" ref="D10:H10" si="0">IF(C10-SUM(D4:D9)&gt;0,C10-SUM(D4:D9),0)</f>
-        <v>2.5</v>
-      </c>
-      <c r="E10" s="16">
+      <c r="B11" s="54">
+        <f>SUM(B4:B10)</f>
+        <v>16</v>
+      </c>
+      <c r="C11" s="16">
+        <f t="shared" ref="C11:H11" si="0">IF(B11-SUM(C4:C10)&gt;0,B11-SUM(C4:C10),0)</f>
+        <v>8</v>
+      </c>
+      <c r="D11" s="16">
         <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="F10" s="16">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="G10" s="16">
+        <v>4.75</v>
+      </c>
+      <c r="E11" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="17">
+      <c r="F11" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I10" s="34" t="s">
+      <c r="G11" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="34" t="s">
+      <c r="J11" s="34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="55">
-        <f>B10</f>
-        <v>12.5</v>
-      </c>
-      <c r="C11" s="19">
-        <f t="shared" ref="C11:H11" si="1">B11-($B$11/COUNTA($C$3:$H$3))</f>
-        <v>10.416666666666666</v>
-      </c>
-      <c r="D11" s="19">
+      <c r="B12" s="55">
+        <f>B11</f>
+        <v>16</v>
+      </c>
+      <c r="C12" s="19">
+        <f t="shared" ref="C12:H12" si="1">B12-($B$12/COUNTA($C$3:$H$3))</f>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="D12" s="19">
         <f t="shared" si="1"/>
-        <v>8.3333333333333321</v>
-      </c>
-      <c r="E11" s="19">
+        <v>10.666666666666668</v>
+      </c>
+      <c r="E12" s="19">
         <f t="shared" si="1"/>
-        <v>6.2499999999999982</v>
-      </c>
-      <c r="F11" s="19">
+        <v>8.0000000000000018</v>
+      </c>
+      <c r="F12" s="19">
         <f t="shared" si="1"/>
-        <v>4.1666666666666643</v>
-      </c>
-      <c r="G11" s="19">
+        <v>5.3333333333333357</v>
+      </c>
+      <c r="G12" s="19">
         <f t="shared" si="1"/>
-        <v>2.0833333333333308</v>
-      </c>
-      <c r="H11" s="20">
+        <v>2.6666666666666692</v>
+      </c>
+      <c r="H12" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I11" s="35">
-        <f>SUM(B4:B9)</f>
-        <v>12.5</v>
-      </c>
-      <c r="J11" s="35">
-        <f>SUM(C4:H9)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="50"/>
+      <c r="I12" s="35">
+        <f>SUM(B4:B10)</f>
+        <v>16</v>
+      </c>
+      <c r="J12" s="35">
+        <f>SUM(C4:H10)</f>
+        <v>21.75</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="50"/>
@@ -21549,6 +21649,9 @@
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="50"/>
     </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="50"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:H2"/>
@@ -21562,8 +21665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21574,7 +21677,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>216</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -21585,23 +21688,23 @@
         <v>215</v>
       </c>
       <c r="E3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="B4" s="63">
-        <v>24</v>
+      <c r="B4">
+        <v>27</v>
       </c>
       <c r="C4" s="62">
-        <f>SUM('Sprint 0'!C4:C10)+SUM('Sprint 1'!H8,'Sprint 1'!C3,'Sprint 1'!C4)+'Sprint 2'!I4+SUM('Sprint 8'!H6:H9,'Sprint 8'!G4:G5)+'Sprint 9'!G14+'Sprint 11'!$C$4+SUM('Sprint 12'!$E$4:$E$5,'Sprint 12'!$C$6:$F$6,'Sprint 12'!$F$7,'Sprint 12'!$F$8:$H$8)</f>
-        <v>45.200001</v>
-      </c>
-      <c r="E4" s="64">
+        <f>SUM('Sprint 0'!C4:C10)+SUM('Sprint 1'!H8,'Sprint 1'!C3,'Sprint 1'!C4)+'Sprint 2'!I4+SUM('Sprint 8'!H6:H9,'Sprint 8'!G4:G5)+'Sprint 9'!G14+'Sprint 11'!$C$4+SUM('Sprint 12'!$E$4:$E$5,'Sprint 12'!$C$6:$F$6,'Sprint 12'!$F$7,'Sprint 12'!$F$8:$H$8)+SUM('Sprint 13'!$C$5,'Sprint 13'!$D$6:$E$6,'Sprint 13'!$F$10:$G$10)</f>
+        <v>63.200001</v>
+      </c>
+      <c r="E4" s="63">
         <f>C4/$C$9</f>
-        <v>0.23547799304257364</v>
+        <v>0.29678328576293361</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -21609,15 +21712,15 @@
         <v>211</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="62">
-        <f>'Sprint 9'!G13+SUM('Sprint 11'!$F$9,'Sprint 11'!$F$8)</f>
-        <v>7</v>
-      </c>
-      <c r="E5" s="64">
+        <f>'Sprint 9'!G13+SUM('Sprint 11'!$F$9,'Sprint 11'!$F$8)+SUM('Sprint 13'!D7:E7)</f>
+        <v>8</v>
+      </c>
+      <c r="E5" s="63">
         <f t="shared" ref="E5:E7" si="0">C5/$C$9</f>
-        <v>3.6467829974119147E-2</v>
+        <v>3.7567503932531096E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -21625,15 +21728,15 @@
         <v>212</v>
       </c>
       <c r="B6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="62">
-        <f>'Sprint 1'!I9+'Sprint 8'!I11+SUM('Sprint 9'!D4,'Sprint 9'!D5,'Sprint 9'!E9,'Sprint 9'!E10,'Sprint 9'!G12)+SUM('Sprint 11'!$F$8,'Sprint 11'!$D$5)+'Sprint 12'!$H$9</f>
-        <v>15.75</v>
-      </c>
-      <c r="E6" s="64">
+        <f>'Sprint 1'!I9+'Sprint 8'!I11+SUM('Sprint 9'!D4,'Sprint 9'!D5,'Sprint 9'!E9,'Sprint 9'!E10,'Sprint 9'!G12)+SUM('Sprint 11'!$F$8,'Sprint 11'!$D$5)+'Sprint 12'!$H$9+'Sprint 13'!$E$9</f>
+        <v>16.75</v>
+      </c>
+      <c r="E6" s="63">
         <f t="shared" si="0"/>
-        <v>8.2052617441768089E-2</v>
+        <v>7.8656961358736982E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -21641,25 +21744,25 @@
         <v>213</v>
       </c>
       <c r="B7">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C7" s="62">
-        <f>SUM('Sprint 1'!F5,'Sprint 1'!I9,'Sprint 1'!I12,'Sprint 1'!I11,'Sprint 1'!I10,'Sprint 1'!F7,'Sprint 1'!F6)+SUM('Sprint 2'!I5:I8)+SUM('Sprint 3'!E4:E5,'Sprint 3'!F6:F7,'Sprint 3'!H8:H10)+SUM('Sprint 4'!H4:H6)+SUM('Sprint 5'!H4:H5)+SUM('Sprint 6'!R4:R9)+SUM('Sprint 7'!K4:K6,'Sprint 7'!O8:O10,'Sprint 7'!P11:P14)+SUM('Sprint 8'!J12,'Sprint 8'!I10,'Sprint 8'!G5)+SUM('Sprint 9'!K15,'Sprint 9'!E11,'Sprint 9'!E9,'Sprint 9'!E8,'Sprint 9'!D7,'Sprint 9'!D6)+SUM('Sprint 10'!D4:D7)+SUM('Sprint 11'!$G$11,'Sprint 11'!$G$10,'Sprint 11'!$F$7,'Sprint 11'!$D$6)</f>
-        <v>124</v>
-      </c>
-      <c r="E7" s="64">
+        <f>SUM('Sprint 1'!F5,'Sprint 1'!I9,'Sprint 1'!I12,'Sprint 1'!I11,'Sprint 1'!I10,'Sprint 1'!F7,'Sprint 1'!F6)+SUM('Sprint 2'!I5:I8)+SUM('Sprint 3'!E4:E5,'Sprint 3'!F6:F7,'Sprint 3'!H8:H10)+SUM('Sprint 4'!H4:H6)+SUM('Sprint 5'!H4:H5)+SUM('Sprint 6'!R4:R9)+SUM('Sprint 7'!K4:K6,'Sprint 7'!O8:O10,'Sprint 7'!P11:P14)+SUM('Sprint 8'!J12,'Sprint 8'!I10,'Sprint 8'!G5)+SUM('Sprint 9'!K15,'Sprint 9'!E11,'Sprint 9'!E9,'Sprint 9'!E8,'Sprint 9'!D7,'Sprint 9'!D6)+SUM('Sprint 10'!D4:D7)+SUM('Sprint 11'!$G$11,'Sprint 11'!$G$10,'Sprint 11'!$F$7,'Sprint 11'!$D$6)+'Sprint 13'!$C$4</f>
+        <v>125</v>
+      </c>
+      <c r="E7" s="63">
         <f t="shared" si="0"/>
-        <v>0.64600155954153915</v>
+        <v>0.58699224894579838</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="65">
+      <c r="B9" s="64">
         <f>SUM(B4:B7)</f>
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C9" s="62">
         <f>SUM(C4:C7)</f>
-        <v>191.95000099999999</v>
+        <v>212.95000099999999</v>
       </c>
     </row>
   </sheetData>
@@ -21686,16 +21789,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="68"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="73"/>
       <c r="M1" s="1">
         <v>0.25</v>
       </c>
@@ -22049,16 +22152,16 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="68"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="73"/>
       <c r="M2" s="1">
         <v>0.25</v>
       </c>
@@ -22327,16 +22430,16 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="68"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="73"/>
       <c r="M2" s="1">
         <v>0.25</v>
       </c>
@@ -22627,16 +22730,16 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="68"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -22827,16 +22930,16 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="71" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="68"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -23012,25 +23115,25 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="68"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="72"/>
+      <c r="R2" s="73"/>
     </row>
     <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -23432,23 +23535,23 @@
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="40"/>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="71" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="68"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
+      <c r="P2" s="73"/>
     </row>
     <row r="3" spans="1:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
@@ -23935,17 +24038,17 @@
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="71" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="68"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="73"/>
     </row>
     <row r="3" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>

</xml_diff>

<commit_message>
Documentación actualizada, primera aproximación del poster, carátula del CD añadida y archivos innecesarios eliminados.
</commit_message>
<xml_diff>
--- a/doc/latex/Scrum.xlsx
+++ b/doc/latex/Scrum.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16215" windowHeight="7530" firstSheet="7" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16215" windowHeight="7530" firstSheet="8" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 0" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,8 @@
     <sheet name="Sprint 11" sheetId="13" r:id="rId12"/>
     <sheet name="Sprint 12" sheetId="15" r:id="rId13"/>
     <sheet name="Sprint 13" sheetId="16" r:id="rId14"/>
-    <sheet name="Resumen" sheetId="14" r:id="rId15"/>
+    <sheet name="Sprint 14" sheetId="17" r:id="rId15"/>
+    <sheet name="Resumen" sheetId="14" r:id="rId16"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="258">
   <si>
     <t>Elegir el lenguaje de programación</t>
   </si>
@@ -780,6 +781,39 @@
   <si>
     <t>Eliminar defectos de código y vulnerabilidades encontradas por SonarQube.</t>
   </si>
+  <si>
+    <t>Actualizar logo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Completar y actualizar la documentación. </t>
+  </si>
+  <si>
+    <t>Diseñar Poster.</t>
+  </si>
+  <si>
+    <t>Sprint 14 (20/06/17 - 26/06/17)</t>
+  </si>
+  <si>
+    <t>Día 1 (20/06/17)</t>
+  </si>
+  <si>
+    <t>Día 2 (21/06/17)</t>
+  </si>
+  <si>
+    <t>Día 3 (22/06/17)</t>
+  </si>
+  <si>
+    <t>Día 4 (23/06/17)</t>
+  </si>
+  <si>
+    <t>Día 5 (24/06/17)</t>
+  </si>
+  <si>
+    <t>Día 6 (25/06/17)</t>
+  </si>
+  <si>
+    <t>Día 7 (26/06/17)</t>
+  </si>
 </sst>
 </file>
 
@@ -1021,7 +1055,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
@@ -1144,6 +1178,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Énfasis3" xfId="5" builtinId="38"/>
@@ -4710,6 +4745,583 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>Sprint 14</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 14'!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Restante</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 14'!$B$3:$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Total Horas</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Día 1 (20/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Día 2 (21/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Día 3 (22/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Día 4 (23/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Día 5 (24/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Día 6 (25/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Día 7 (26/06/17)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 14'!$B$7:$I$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-62D3-4CEF-BEA6-C2A261B32C4F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 14'!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 14'!$B$3:$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Total Horas</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Día 1 (20/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Día 2 (21/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Día 3 (22/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Día 4 (23/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Día 5 (24/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Día 6 (25/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Día 7 (26/06/17)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 14'!$B$8:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.1428571428571432</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2857142857142865</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4285714285714293</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5714285714285721</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7142857142857149</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.85714285714285776</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-62D3-4CEF-BEA6-C2A261B32C4F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="404108848"/>
+        <c:axId val="404106880"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="404108848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Dias</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="404106880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="404106880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Horas</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="404108848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
               <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="50" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
@@ -4958,16 +5570,16 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.28997476811206807</c:v>
+                  <c:v>0.30984663565304899</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.6705666268843008E-2</c:v>
+                  <c:v>3.5563458388248689E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.9793530168416938E-2</c:v>
+                  <c:v>9.6688152493051113E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57352603545067204</c:v>
+                  <c:v>0.5579017534656513</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10165,6 +10777,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -13504,6 +14156,509 @@
 </file>
 
 <file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="258">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -18569,6 +19724,93 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
+      <xdr:colOff>19053</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19ECD442-CA87-458B-9ADB-39C8A70890EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>433316</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>103905</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01B762DE-6797-4FF4-85A1-43242DB48C95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6143625" y="2133600"/>
+          <a:ext cx="5767316" cy="3151905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -18604,23 +19846,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>698389</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>12589</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>126731</xdr:rowOff>
+      <xdr:rowOff>88631</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71696C5C-79C2-4CB6-B5AD-755BD9288FDE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F02DB9A-1946-4CDD-B7DC-6C313F116BB3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18636,7 +19878,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5048250" y="1943100"/>
+          <a:off x="5124450" y="1905000"/>
           <a:ext cx="4584589" cy="2755631"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -21355,7 +22597,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A2" sqref="A2:K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21703,10 +22945,280 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="69.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="44"/>
+      <c r="B2" s="71" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="73"/>
+    </row>
+    <row r="3" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="41"/>
+      <c r="B3" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>252</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="51">
+        <v>1</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="57" t="s">
+        <v>249</v>
+      </c>
+      <c r="B5" s="65">
+        <v>2</v>
+      </c>
+      <c r="C5" s="66"/>
+      <c r="D5" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="46">
+        <v>1</v>
+      </c>
+      <c r="F5" s="46">
+        <v>2</v>
+      </c>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="47"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="43" t="s">
+        <v>248</v>
+      </c>
+      <c r="B6" s="53">
+        <v>3</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13">
+        <v>2</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13"/>
+      <c r="I6" s="14"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="54">
+        <f>SUM(B4:B6)</f>
+        <v>6</v>
+      </c>
+      <c r="C7" s="16">
+        <f>IF(B7-SUM(C4:C6)&gt;0,B7-SUM(C4:C6),0)</f>
+        <v>5.5</v>
+      </c>
+      <c r="D7" s="16">
+        <f t="shared" ref="D7:I7" si="0">IF(C7-SUM(D4:D6)&gt;0,C7-SUM(D4:D6),0)</f>
+        <v>4</v>
+      </c>
+      <c r="E7" s="16">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F7" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="55">
+        <f>B7</f>
+        <v>6</v>
+      </c>
+      <c r="C8" s="19">
+        <f>B8-($B$8/COUNTA($C$3:$I$3))</f>
+        <v>5.1428571428571432</v>
+      </c>
+      <c r="D8" s="19">
+        <f t="shared" ref="D8:I8" si="1">C8-($B$8/COUNTA($C$3:$I$3))</f>
+        <v>4.2857142857142865</v>
+      </c>
+      <c r="E8" s="19">
+        <f t="shared" si="1"/>
+        <v>3.4285714285714293</v>
+      </c>
+      <c r="F8" s="19">
+        <f t="shared" si="1"/>
+        <v>2.5714285714285721</v>
+      </c>
+      <c r="G8" s="19">
+        <f t="shared" si="1"/>
+        <v>1.7142857142857149</v>
+      </c>
+      <c r="H8" s="19">
+        <f t="shared" si="1"/>
+        <v>0.85714285714285776</v>
+      </c>
+      <c r="I8" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="35">
+        <f>SUM(B4:B6)</f>
+        <v>6</v>
+      </c>
+      <c r="K8" s="35">
+        <f>SUM(C4:I6)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="50"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="50"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="50"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="50"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="50"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="50"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="50"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="50"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="50"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="50"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="50"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="50"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="50"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="50"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="50"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="50"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="50"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="50"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="50"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21736,22 +23248,22 @@
         <v>210</v>
       </c>
       <c r="B4">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C4" s="62">
-        <f>SUM('Sprint 0'!C4:C10)+SUM('Sprint 1'!H8,'Sprint 1'!C3,'Sprint 1'!C4)+'Sprint 2'!I4+SUM('Sprint 8'!H6:H9,'Sprint 8'!G4:G5)+'Sprint 9'!G14+'Sprint 11'!$C$4+SUM('Sprint 12'!$E$4:$E$5,'Sprint 12'!$C$6:$F$6,'Sprint 12'!$F$7,'Sprint 12'!$F$8:$H$8)+SUM('Sprint 13'!$C$5,'Sprint 13'!$D$6:$E$6,'Sprint 13'!$F$10:$G$10)</f>
-        <v>63.200001</v>
+        <f>SUM('Sprint 0'!C4:C10)+SUM('Sprint 1'!H8,'Sprint 1'!C3,'Sprint 1'!C4)+'Sprint 2'!I4+SUM('Sprint 8'!H6:H9,'Sprint 8'!G4:G5)+'Sprint 9'!G14+'Sprint 11'!$C$4+SUM('Sprint 12'!$E$4:$E$5,'Sprint 12'!$C$6:$F$6,'Sprint 12'!$F$7,'Sprint 12'!$F$8:$H$8)+SUM('Sprint 13'!$C$5,'Sprint 13'!$D$6:$E$6,'Sprint 13'!$F$10:$G$10)+SUM('Sprint 14'!D5:F5,'Sprint 14'!F6:G6)</f>
+        <v>69.700001</v>
       </c>
       <c r="E4" s="63">
         <f>C4/$C$9</f>
-        <v>0.28997476811206807</v>
+        <v>0.30984663565304899</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="74">
         <v>4</v>
       </c>
       <c r="C5" s="62">
@@ -21760,7 +23272,7 @@
       </c>
       <c r="E5" s="63">
         <f t="shared" ref="E5:E7" si="0">C5/$C$9</f>
-        <v>3.6705666268843008E-2</v>
+        <v>3.5563458388248689E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -21776,7 +23288,7 @@
       </c>
       <c r="E6" s="63">
         <f t="shared" si="0"/>
-        <v>9.9793530168416938E-2</v>
+        <v>9.6688152493051113E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -21784,30 +23296,31 @@
         <v>213</v>
       </c>
       <c r="B7">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C7" s="62">
-        <f>SUM('Sprint 1'!F5,'Sprint 1'!I9,'Sprint 1'!I12,'Sprint 1'!I11,'Sprint 1'!I10,'Sprint 1'!F7,'Sprint 1'!F6)+SUM('Sprint 2'!I5:I8)+SUM('Sprint 3'!E4:E5,'Sprint 3'!F6:F7,'Sprint 3'!H8:H10)+SUM('Sprint 4'!H4:H6)+SUM('Sprint 5'!H4:H5)+SUM('Sprint 6'!R4:R9)+SUM('Sprint 7'!K4:K6,'Sprint 7'!O8:O10,'Sprint 7'!P11:P14)+SUM('Sprint 8'!J12,'Sprint 8'!I10,'Sprint 8'!G5)+SUM('Sprint 9'!K15,'Sprint 9'!E11,'Sprint 9'!E9,'Sprint 9'!E8,'Sprint 9'!D7,'Sprint 9'!D6)+SUM('Sprint 10'!D4:D7)+SUM('Sprint 11'!$G$11,'Sprint 11'!$G$10,'Sprint 11'!$F$7,'Sprint 11'!$D$6)+'Sprint 13'!$C$4</f>
-        <v>125</v>
+        <f>SUM('Sprint 1'!F5,'Sprint 1'!I9,'Sprint 1'!I12,'Sprint 1'!I11,'Sprint 1'!I10,'Sprint 1'!F7,'Sprint 1'!F6)+SUM('Sprint 2'!I5:I8)+SUM('Sprint 3'!E4:E5,'Sprint 3'!F6:F7,'Sprint 3'!H8:H10)+SUM('Sprint 4'!H4:H6)+SUM('Sprint 5'!H4:H5)+SUM('Sprint 6'!R4:R9)+SUM('Sprint 7'!K4:K6,'Sprint 7'!O8:O10,'Sprint 7'!P11:P14)+SUM('Sprint 8'!J12,'Sprint 8'!I10,'Sprint 8'!G5)+SUM('Sprint 9'!K15,'Sprint 9'!E11,'Sprint 9'!E9,'Sprint 9'!E8,'Sprint 9'!D7,'Sprint 9'!D6)+SUM('Sprint 10'!D4:D7)+SUM('Sprint 11'!$G$11,'Sprint 11'!$G$10,'Sprint 11'!$F$7,'Sprint 11'!$D$6)+'Sprint 13'!$C$4+'Sprint 14'!C4:D4</f>
+        <v>125.5</v>
       </c>
       <c r="E7" s="63">
         <f t="shared" si="0"/>
-        <v>0.57352603545067204</v>
+        <v>0.5579017534656513</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="64">
-        <f>109</f>
-        <v>109</v>
+        <f>112</f>
+        <v>112</v>
       </c>
       <c r="C9" s="62">
         <f>SUM(C4:C7)</f>
-        <v>217.95000099999999</v>
+        <v>224.95000099999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Versión final de la documentación y el cartel.
</commit_message>
<xml_diff>
--- a/doc/latex/Scrum.xlsx
+++ b/doc/latex/Scrum.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16215" windowHeight="7530" firstSheet="8" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16215" windowHeight="7530" firstSheet="9" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 0" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,8 @@
     <sheet name="Sprint 12" sheetId="15" r:id="rId13"/>
     <sheet name="Sprint 13" sheetId="16" r:id="rId14"/>
     <sheet name="Sprint 14" sheetId="17" r:id="rId15"/>
-    <sheet name="Resumen" sheetId="14" r:id="rId16"/>
+    <sheet name="Sprint 15" sheetId="18" r:id="rId16"/>
+    <sheet name="Resumen" sheetId="14" r:id="rId17"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="270">
   <si>
     <t>Elegir el lenguaje de programación</t>
   </si>
@@ -814,6 +815,42 @@
   <si>
     <t>Día 7 (26/06/17)</t>
   </si>
+  <si>
+    <t>Actualizar la documentación y el póster a su versión final.</t>
+  </si>
+  <si>
+    <t>Crear máquina virtual para ejecutar rápidamente la aplicación.</t>
+  </si>
+  <si>
+    <t>Sprint 15 (27/06/17 - 03/07/17)</t>
+  </si>
+  <si>
+    <t>Día 1 (27/06/17)</t>
+  </si>
+  <si>
+    <t>Día 2 (28/06/17)</t>
+  </si>
+  <si>
+    <t>Día 3 (29/06/17)</t>
+  </si>
+  <si>
+    <t>Día 4 (30/06/17)</t>
+  </si>
+  <si>
+    <t>Día 5 (01/07/17)</t>
+  </si>
+  <si>
+    <t>Día 6 (02/07/17)</t>
+  </si>
+  <si>
+    <t>Día 7 (03/07/17)</t>
+  </si>
+  <si>
+    <t>Grabar los discos.</t>
+  </si>
+  <si>
+    <t>Realizar entrega.</t>
+  </si>
 </sst>
 </file>
 
@@ -1055,7 +1092,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
@@ -1169,6 +1206,7 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="10" borderId="10" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1178,7 +1216,16 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="1" fillId="9" borderId="7" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="9" borderId="7" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="9" borderId="8" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Énfasis3" xfId="5" builtinId="38"/>
@@ -5322,6 +5369,583 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>Sprint 15</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 15'!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Restante</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 15'!$B$3:$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Total Horas</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Día 1 (27/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Día 2 (28/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Día 3 (29/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Día 4 (30/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Día 5 (01/07/17)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Día 6 (02/07/17)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Día 7 (03/07/17)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 15'!$B$8:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-460B-4276-BB71-EFEF44EAD79E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 15'!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 15'!$B$3:$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Total Horas</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Día 1 (27/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Día 2 (28/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Día 3 (29/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Día 4 (30/06/17)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Día 5 (01/07/17)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Día 6 (02/07/17)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Día 7 (03/07/17)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 15'!$B$9:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-460B-4276-BB71-EFEF44EAD79E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="404108848"/>
+        <c:axId val="404106880"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="404108848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Dias</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="404106880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="404106880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Horas</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="404108848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
               <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="50" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
@@ -5570,16 +6194,16 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.30984663565304899</c:v>
+                  <c:v>0.32704811735133027</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5563458388248689E-2</c:v>
+                  <c:v>3.4677069637290552E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.6688152493051113E-2</c:v>
+                  <c:v>9.4278283076383695E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5579017534656513</c:v>
+                  <c:v>0.54399652993499559</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10817,6 +11441,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -14659,6 +15323,509 @@
 </file>
 
 <file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="258">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -19811,6 +20978,93 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
+      <xdr:colOff>19053</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A8E01FD-4001-4BDC-9B54-46DAFA25B867}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>366188</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>110002</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73532E57-DD24-4E8B-AA02-491D6FD3AF30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5314950" y="2324100"/>
+          <a:ext cx="4938188" cy="3158002"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -19859,10 +21113,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
+        <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F02DB9A-1946-4CDD-B7DC-6C313F116BB3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B346BBDE-2EBF-4861-9D08-733AEC60A117}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20901,16 +22155,16 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="74"/>
       <c r="L2" s="3">
         <v>1</v>
       </c>
@@ -21241,18 +22495,18 @@
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="72" t="s">
         <v>175</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="74"/>
     </row>
     <row r="3" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
@@ -21648,22 +22902,22 @@
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="72" t="s">
         <v>177</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="72"/>
-      <c r="O2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="74"/>
     </row>
     <row r="3" spans="1:15" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
@@ -21970,15 +23224,15 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="72" t="s">
         <v>199</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="74"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
@@ -22303,15 +23557,15 @@
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="72" t="s">
         <v>218</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
@@ -22608,15 +23862,15 @@
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="72" t="s">
         <v>231</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="74"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
@@ -22947,8 +24201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection sqref="A1:K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22959,16 +24213,16 @@
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="72" t="s">
         <v>250</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="74"/>
     </row>
     <row r="3" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
@@ -23215,10 +24469,286 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="44"/>
+      <c r="B2" s="72" t="s">
+        <v>260</v>
+      </c>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="74"/>
+    </row>
+    <row r="3" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="41"/>
+      <c r="B3" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="56" t="s">
+        <v>258</v>
+      </c>
+      <c r="B4" s="51">
+        <v>2.5</v>
+      </c>
+      <c r="C4" s="10">
+        <v>3</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="57" t="s">
+        <v>259</v>
+      </c>
+      <c r="B5" s="65">
+        <v>1.5</v>
+      </c>
+      <c r="C5" s="66">
+        <v>1.5</v>
+      </c>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="47"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="67" t="s">
+        <v>268</v>
+      </c>
+      <c r="B6" s="68">
+        <v>0.75</v>
+      </c>
+      <c r="C6" s="75"/>
+      <c r="D6" s="69">
+        <v>0.75</v>
+      </c>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="77"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="78" t="s">
+        <v>269</v>
+      </c>
+      <c r="B7" s="79">
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="80"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="82">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="54">
+        <f>SUM(B4:B7)</f>
+        <v>5.25</v>
+      </c>
+      <c r="C8" s="16">
+        <f>IF(B8-SUM(C4:C7)&gt;0,B8-SUM(C4:C7),0)</f>
+        <v>0.75</v>
+      </c>
+      <c r="D8" s="16">
+        <f t="shared" ref="D8:I8" si="0">IF(C8-SUM(D4:D7)&gt;0,C8-SUM(D4:D7),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="16">
+        <f>IF(H8-SUM(I4:I7)&gt;0,H8-SUM(I4:I7),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="55">
+        <f>B8</f>
+        <v>5.25</v>
+      </c>
+      <c r="C9" s="19">
+        <f>B9-($B$9/COUNTA($C$3:$I$3))</f>
+        <v>4.5</v>
+      </c>
+      <c r="D9" s="19">
+        <f t="shared" ref="D9:I9" si="1">C9-($B$9/COUNTA($C$3:$I$3))</f>
+        <v>3.75</v>
+      </c>
+      <c r="E9" s="19">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F9" s="19">
+        <f t="shared" si="1"/>
+        <v>2.25</v>
+      </c>
+      <c r="G9" s="19">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="H9" s="19">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="I9" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="35">
+        <f>SUM(B4:B7)</f>
+        <v>5.25</v>
+      </c>
+      <c r="K9" s="35">
+        <f>SUM(C4:I7)</f>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="50"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="50"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="50"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="50"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="50"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="50"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="50"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="50"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="50"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="50"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="50"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="50"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="50"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="50"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="50"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="50"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="50"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="50"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23248,22 +24778,22 @@
         <v>210</v>
       </c>
       <c r="B4">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C4" s="62">
-        <f>SUM('Sprint 0'!C4:C10)+SUM('Sprint 1'!H8,'Sprint 1'!C3,'Sprint 1'!C4)+'Sprint 2'!I4+SUM('Sprint 8'!H6:H9,'Sprint 8'!G4:G5)+'Sprint 9'!G14+'Sprint 11'!$C$4+SUM('Sprint 12'!$E$4:$E$5,'Sprint 12'!$C$6:$F$6,'Sprint 12'!$F$7,'Sprint 12'!$F$8:$H$8)+SUM('Sprint 13'!$C$5,'Sprint 13'!$D$6:$E$6,'Sprint 13'!$F$10:$G$10)+SUM('Sprint 14'!D5:F5,'Sprint 14'!F6:G6)</f>
-        <v>69.700001</v>
+        <f>SUM('Sprint 0'!C4:C10)+SUM('Sprint 1'!H8,'Sprint 1'!C3,'Sprint 1'!C4)+'Sprint 2'!I4+SUM('Sprint 8'!H6:H9,'Sprint 8'!G4:G5)+'Sprint 9'!G14+'Sprint 11'!$C$4+SUM('Sprint 12'!$E$4:$E$5,'Sprint 12'!$C$6:$F$6,'Sprint 12'!$F$7,'Sprint 12'!$F$8:$H$8)+SUM('Sprint 13'!$C$5,'Sprint 13'!$D$6:$E$6,'Sprint 13'!$F$10:$G$10)+SUM('Sprint 14'!D5:F5,'Sprint 14'!F6:G6)+SUM('Sprint 15'!C4:C5,'Sprint 15'!D6,'Sprint 15'!I7)</f>
+        <v>75.450001</v>
       </c>
       <c r="E4" s="63">
         <f>C4/$C$9</f>
-        <v>0.30984663565304899</v>
+        <v>0.32704811735133027</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="B5" s="74">
+      <c r="B5" s="71">
         <v>4</v>
       </c>
       <c r="C5" s="62">
@@ -23272,7 +24802,7 @@
       </c>
       <c r="E5" s="63">
         <f t="shared" ref="E5:E7" si="0">C5/$C$9</f>
-        <v>3.5563458388248689E-2</v>
+        <v>3.4677069637290552E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -23288,7 +24818,7 @@
       </c>
       <c r="E6" s="63">
         <f t="shared" si="0"/>
-        <v>9.6688152493051113E-2</v>
+        <v>9.4278283076383695E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -23304,17 +24834,17 @@
       </c>
       <c r="E7" s="63">
         <f t="shared" si="0"/>
-        <v>0.5579017534656513</v>
+        <v>0.54399652993499559</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="64">
-        <f>112</f>
-        <v>112</v>
+        <f>116</f>
+        <v>116</v>
       </c>
       <c r="C9" s="62">
         <f>SUM(C4:C7)</f>
-        <v>224.95000099999999</v>
+        <v>230.70000099999999</v>
       </c>
     </row>
   </sheetData>
@@ -23342,16 +24872,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="74"/>
       <c r="M1" s="1">
         <v>0.25</v>
       </c>
@@ -23705,16 +25235,16 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="74"/>
       <c r="M2" s="1">
         <v>0.25</v>
       </c>
@@ -23983,16 +25513,16 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="74"/>
       <c r="M2" s="1">
         <v>0.25</v>
       </c>
@@ -24283,16 +25813,16 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="74"/>
     </row>
     <row r="3" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -24483,16 +26013,16 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="74"/>
     </row>
     <row r="3" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -24668,25 +26198,25 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="72"/>
-      <c r="O2" s="72"/>
-      <c r="P2" s="72"/>
-      <c r="Q2" s="72"/>
-      <c r="R2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="74"/>
     </row>
     <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -25088,23 +26618,23 @@
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="40"/>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="72" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="72"/>
-      <c r="O2" s="72"/>
-      <c r="P2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="74"/>
     </row>
     <row r="3" spans="1:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
@@ -25591,17 +27121,17 @@
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="72" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="74"/>
     </row>
     <row r="3" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>

</xml_diff>